<commit_message>
sam aan het werk
</commit_message>
<xml_diff>
--- a/resultaten/Opgave B/OpgaveB_resultaten.xlsx
+++ b/resultaten/Opgave B/OpgaveB_resultaten.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1ACB4F-11C4-444F-8371-36F358ED80C2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEB0B34B-D7B0-4824-85A9-9B1A9E666E9B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,6 +11,7 @@
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -110,9 +111,6 @@
   </si>
   <si>
     <t>Run_time</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Capaciteits-Greedy + RandomHillclimber*</t>
@@ -502,7 +500,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +533,7 @@
         <v>27</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
@@ -692,9 +690,6 @@
       <c r="E8" s="7">
         <v>0</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
@@ -713,7 +708,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="8">
         <v>1</v>
@@ -763,7 +758,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="8">
         <v>1</v>
@@ -892,7 +887,7 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="8">
         <v>2</v>
@@ -928,10 +923,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" s="8">
         <v>1</v>
@@ -948,7 +943,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" s="8">
         <v>2</v>
@@ -965,7 +960,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28" s="8">
         <v>3</v>

</xml_diff>